<commit_message>
Implemented loggers in extent report
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,19 +4,24 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="MensPant" sheetId="2" r:id="rId2"/>
     <sheet name="MensTop" sheetId="3" r:id="rId3"/>
+    <sheet name="WomensPant" sheetId="4" r:id="rId4"/>
+    <sheet name="WomensTops" sheetId="5" r:id="rId5"/>
+    <sheet name="Outerwear" sheetId="6" r:id="rId6"/>
+    <sheet name="Skirts" sheetId="7" r:id="rId7"/>
+    <sheet name="Scarves" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="54">
   <si>
     <t>Username</t>
   </si>
@@ -109,6 +114,75 @@
   </si>
   <si>
     <t>Linda</t>
+  </si>
+  <si>
+    <t>CouponCode</t>
+  </si>
+  <si>
+    <t>LucasSBaty@dayrep.com</t>
+  </si>
+  <si>
+    <t>Ali-Ra Clean Cut Skinny Jeans</t>
+  </si>
+  <si>
+    <t>GPAS</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>CiaraDShue@armyspy.com</t>
+  </si>
+  <si>
+    <t>OCeanWater Reef Women's Jeans</t>
+  </si>
+  <si>
+    <t>Ciara</t>
+  </si>
+  <si>
+    <t>AshleyTDevore@jourrapide.com</t>
+  </si>
+  <si>
+    <t>Ali-Ra Alternating Striped Blouse</t>
+  </si>
+  <si>
+    <t>Ashley</t>
+  </si>
+  <si>
+    <t>JosephFZimmerman@superrito.com</t>
+  </si>
+  <si>
+    <t>Gabardine BunchedUp Blouse</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>DonaldMDaves@fleckens.hu</t>
+  </si>
+  <si>
+    <t>Dad Hat</t>
+  </si>
+  <si>
+    <t>Donald</t>
+  </si>
+  <si>
+    <t>HelenDJackson@gustr.com</t>
+  </si>
+  <si>
+    <t>X-Press Pleated A-Line</t>
+  </si>
+  <si>
+    <t>Helen</t>
+  </si>
+  <si>
+    <t>NicoleJHartmann@einrot.com</t>
+  </si>
+  <si>
+    <t>Fyre Hand-knit Infinity</t>
+  </si>
+  <si>
+    <t>Nicole</t>
   </si>
 </sst>
 </file>
@@ -118,8 +192,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -132,7 +206,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,8 +218,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,10 +240,73 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -173,9 +318,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,77 +333,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,7 +348,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,19 +363,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,163 +537,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,41 +568,6 @@
       </top>
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -589,6 +628,41 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -598,7 +672,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -616,143 +690,146 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1130,7 +1207,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="7"/>
@@ -1195,7 +1272,7 @@
       </c>
     </row>
     <row r="3" ht="15.15" spans="1:8">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1234,8 +1311,8 @@
   <sheetPr/>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -1277,7 +1354,7 @@
       </c>
     </row>
     <row r="2" ht="15.15" spans="1:9">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1306,7 +1383,7 @@
       </c>
     </row>
     <row r="3" ht="15.15" spans="1:9">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1321,7 +1398,7 @@
       <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="G3" t="s">
@@ -1342,4 +1419,462 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="30.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="15.2222222222222" customWidth="1"/>
+    <col min="3" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="17.8888888888889" customWidth="1"/>
+    <col min="6" max="6" width="18.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.15" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" ht="15.15" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2">
+        <v>1023</v>
+      </c>
+      <c r="I2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" ht="15.15" spans="1:9">
+      <c r="A3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3">
+        <v>1123</v>
+      </c>
+      <c r="I3">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="CiaraDShue@armyspy.com" tooltip="mailto:CiaraDShue@armyspy.com"/>
+    <hyperlink ref="A2" r:id="rId2" display="LucasSBaty@dayrep.com" tooltip="mailto:LucasSBaty@dayrep.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="30.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="15.2222222222222" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="17.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="18.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.15" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" ht="15.15" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2">
+        <v>1023</v>
+      </c>
+      <c r="H2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" ht="15.15" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3">
+        <v>1123</v>
+      </c>
+      <c r="H3">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="JosephFZimmerman@superrito.com" tooltip="mailto:JosephFZimmerman@superrito.com"/>
+    <hyperlink ref="A2" r:id="rId2" display="AshleyTDevore@jourrapide.com" tooltip="mailto:AshleyTDevore@jourrapide.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="30.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="15.2222222222222" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="17.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="18.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.15" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" ht="15.15" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2">
+        <v>1023</v>
+      </c>
+      <c r="H2">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="DonaldMDaves@fleckens.hu" tooltip="mailto:DonaldMDaves@fleckens.hu"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="30.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="15.2222222222222" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="17.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="18.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.15" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>1023</v>
+      </c>
+      <c r="H2">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="HelenDJackson@gustr.com" tooltip="mailto:HelenDJackson@gustr.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="30.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="15.2222222222222" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="17.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="18.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.15" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" ht="15.15" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2">
+        <v>1023</v>
+      </c>
+      <c r="H2">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="NicoleJHartmann@einrot.com" tooltip="mailto:NicoleJHartmann@einrot.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>